<commit_message>
updated bug bash list
</commit_message>
<xml_diff>
--- a/Bug Bash/Team13-Issue Report.xlsx
+++ b/Bug Bash/Team13-Issue Report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="156">
   <si>
     <t>Team Number</t>
   </si>
@@ -511,6 +511,53 @@
   </si>
   <si>
     <t xml:space="preserve">An error message popup indicating access is denied when accessing  some protected system files </t>
+  </si>
+  <si>
+    <t>System reports "We are done synchronizing" but no files are copied to Tzync folder in the exe root folder (For first time sync on the first computer)</t>
+  </si>
+  <si>
+    <t>Inappropriate error message is displayed when changing the root folder (for first time sync on the first computer)</t>
+  </si>
+  <si>
+    <t>System displays inappropriate error message when sync is clicked (For first time sync on the first computer)</t>
+  </si>
+  <si>
+    <t>Select a root folder by drag &amp; drop. 
+Then change the root folder using drag &amp; drop again. A error message "An error has occurred while loading data! Please choose the correct sync folder." is displayed.
+This does not happen if I use the "Browse" button to change the root folder</t>
+  </si>
+  <si>
+    <t>Select a folder to sync on the first computer.
+Change to another folder using "Browse button".
+Click on Sync button.
+Click OK when confirmation dialog boxes appear.
+System reports "We are done synchronizing" but no files are copied to the Tzync folder.</t>
+  </si>
+  <si>
+    <t>Select a folder to sync on the first computer.
+Change to another folder using "Browse button".
+Click on Sync button.
+Click OK for 2 times.
+System display error message "Please choose a valid folder" while the folder input is a valid directory.</t>
+  </si>
+  <si>
+    <t>Create a folder named "A".
+Create another folder named "A1" with B as its sub-folder.
+Select folder "A" as source, then select "A1\B" as destination directory</t>
+  </si>
+  <si>
+    <t>System displays "Folders that are to be synchronized cannot be a subdirectory of each other" where the source and destination folders are not sub-directory of each other</t>
+  </si>
+  <si>
+    <t>Not able to setup sync for the second computer after sync has been sucessfully performed on the first computer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select a root folder to sync on the first computer.
+Click Sync.
+Then save the Tzsync folder and the executable on a USB device.
+Go to the second computer and run the exe.
+Select a folder on the second computer to sync. 
+System displays "Ouch that hurts. Don't do this again" and terminates </t>
   </si>
 </sst>
 </file>
@@ -916,16 +963,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="41.5703125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" style="7" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="49.28515625" style="7" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
@@ -1254,698 +1299,698 @@
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="45">
+    <row r="20" spans="1:5" s="2" customFormat="1" ht="105">
       <c r="A20" s="3">
         <v>4</v>
       </c>
       <c r="B20" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="2" customFormat="1" ht="90">
+      <c r="A21" s="3">
+        <v>4</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="2" customFormat="1" ht="90">
+      <c r="A22" s="3">
+        <v>4</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="2" customFormat="1" ht="120">
+      <c r="A23" s="3">
+        <v>4</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="45">
+      <c r="A24" s="3">
+        <v>4</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="8" t="s">
+      <c r="C24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E24" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="90">
-      <c r="A21" s="3">
-        <v>5</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="90">
-      <c r="A22" s="3">
-        <v>5</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="90">
-      <c r="A23" s="3">
-        <v>5</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="2" customFormat="1" ht="30">
-      <c r="A24" s="3">
-        <v>5</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="45">
+    <row r="25" spans="1:5" ht="90">
       <c r="A25" s="3">
         <v>5</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="8" t="s">
+      <c r="B25" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E25" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="2" customFormat="1" ht="30">
+    <row r="26" spans="1:5" ht="90">
       <c r="A26" s="3">
         <v>5</v>
       </c>
-      <c r="B26" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" s="2" customFormat="1" ht="75">
+      <c r="B26" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="90">
       <c r="A27" s="3">
         <v>5</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>143</v>
+        <v>67</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="8" t="s">
-        <v>144</v>
+      <c r="D27" s="10" t="s">
+        <v>68</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="90">
+    <row r="28" spans="1:5" s="2" customFormat="1" ht="30">
       <c r="A28" s="3">
+        <v>5</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="7" t="s">
+      <c r="D28" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E28" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="75">
+    <row r="29" spans="1:5" ht="45">
       <c r="A29" s="3">
-        <v>7</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="75">
+    <row r="30" spans="1:5" s="2" customFormat="1" ht="30">
       <c r="A30" s="3">
-        <v>7</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="90">
+        <v>5</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="2" customFormat="1" ht="75">
       <c r="A31" s="3">
-        <v>7</v>
-      </c>
-      <c r="B31" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="105">
+      <c r="B31" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="90">
       <c r="A32" s="3">
         <v>7</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>12</v>
+        <v>104</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>106</v>
+        <v>9</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="45">
+    <row r="33" spans="1:5" ht="75">
       <c r="A33" s="3">
+        <v>7</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C33" s="5" t="s">
+    </row>
+    <row r="34" spans="1:5" ht="75">
+      <c r="A34" s="3">
         <v>7</v>
       </c>
-      <c r="D33" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="90">
-      <c r="A34" s="3">
+      <c r="B34" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="E34" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="60">
+    </row>
+    <row r="35" spans="1:5" ht="90">
       <c r="A35" s="3">
+        <v>7</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B35" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="120">
+    </row>
+    <row r="36" spans="1:5" ht="105">
       <c r="A36" s="3">
+        <v>7</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E36" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B36" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="75">
+    </row>
+    <row r="37" spans="1:5" ht="45">
       <c r="A37" s="3">
         <v>8</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="E37" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="135">
+    <row r="38" spans="1:5" ht="90">
       <c r="A38" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>140</v>
+        <v>72</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D38" s="10" t="s">
-        <v>82</v>
+      <c r="D38" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="75">
+    <row r="39" spans="1:5" ht="60">
       <c r="A39" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="90">
+    <row r="40" spans="1:5" ht="120">
       <c r="A40" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D40" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E40" s="8" t="s">
+      <c r="D40" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E40" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="105">
+    <row r="41" spans="1:5" ht="75">
       <c r="A41" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>139</v>
+        <v>80</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E41" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E41" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="60">
+    <row r="42" spans="1:5" ht="135">
       <c r="A42" s="3">
         <v>9</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>88</v>
+        <v>140</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D42" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E42" s="7" t="s">
+      <c r="D42" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E42" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="60">
+    <row r="43" spans="1:5" ht="75">
       <c r="A43" s="3">
         <v>9</v>
       </c>
       <c r="B43" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="90">
+      <c r="A44" s="3">
+        <v>9</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="105">
+      <c r="A45" s="3">
+        <v>9</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="60">
+      <c r="A46" s="3">
+        <v>9</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="60">
+      <c r="A47" s="3">
+        <v>9</v>
+      </c>
+      <c r="B47" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C43" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="8" t="s">
+      <c r="C47" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="E43" s="7" t="s">
+      <c r="E47" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="15" customFormat="1" ht="30">
-      <c r="A44" s="3">
-        <v>10</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="E44" s="15" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" s="15" customFormat="1">
-      <c r="A45" s="3">
-        <v>10</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="E45" s="15" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" s="15" customFormat="1" ht="30">
-      <c r="A46" s="3">
-        <v>10</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="E46" s="15" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" s="15" customFormat="1" ht="60">
-      <c r="A47" s="3">
-        <v>10</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="E47" s="15" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" s="15" customFormat="1" ht="45">
+    <row r="48" spans="1:5" s="15" customFormat="1" ht="30">
       <c r="A48" s="3">
         <v>10</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>111</v>
+        <v>141</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="E48" s="15" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="15" customFormat="1" ht="45">
+    <row r="49" spans="1:5" s="15" customFormat="1">
       <c r="A49" s="3">
         <v>10</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="E49" s="15" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="15" customFormat="1" ht="45">
+    <row r="50" spans="1:5" s="15" customFormat="1" ht="30">
       <c r="A50" s="3">
         <v>10</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="E50" s="15" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="15" customFormat="1" ht="45">
+    <row r="51" spans="1:5" s="15" customFormat="1" ht="60">
       <c r="A51" s="3">
         <v>10</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E51" s="15" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="15" customFormat="1">
+    <row r="52" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="A52" s="3">
         <v>10</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E52" s="15" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="15" customFormat="1" ht="30">
+    <row r="53" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="A53" s="3">
         <v>10</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="E53" s="15" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="15" customFormat="1" ht="30">
+    <row r="54" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="A54" s="3">
         <v>10</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E54" s="15" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="75">
+    <row r="55" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="A55" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>13</v>
+        <v>116</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E55" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="60">
+        <v>117</v>
+      </c>
+      <c r="E55" s="15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="15" customFormat="1">
       <c r="A56" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>16</v>
+        <v>118</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E56" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="60">
+        <v>119</v>
+      </c>
+      <c r="E56" s="15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="15" customFormat="1" ht="30">
       <c r="A57" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>18</v>
+        <v>120</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E57" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="75">
+        <v>121</v>
+      </c>
+      <c r="E57" s="15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="15" customFormat="1" ht="30">
       <c r="A58" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>20</v>
+        <v>122</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E58" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="60">
+        <v>123</v>
+      </c>
+      <c r="E58" s="15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="75">
       <c r="A59" s="3">
         <v>11</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E59" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="75">
+    <row r="60" spans="1:5" ht="60">
       <c r="A60" s="3">
         <v>11</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E60" s="8" t="s">
         <v>15</v>
@@ -1956,13 +2001,13 @@
         <v>11</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E61" s="8" t="s">
         <v>15</v>
@@ -1973,151 +2018,236 @@
         <v>11</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="90">
+    <row r="63" spans="1:5" ht="60">
       <c r="A63" s="3">
         <v>11</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D63" s="10" t="s">
-        <v>31</v>
+        <v>7</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="E63" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="150">
+    <row r="64" spans="1:5" ht="75">
       <c r="A64" s="3">
         <v>11</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D64" s="10" t="s">
-        <v>33</v>
+      <c r="D64" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="75">
+    <row r="65" spans="1:5" ht="60">
       <c r="A65" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E65" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="90">
+    <row r="66" spans="1:5" ht="75">
       <c r="A66" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D66" s="12" t="s">
-        <v>37</v>
+      <c r="D66" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="75">
+    <row r="67" spans="1:5" ht="90">
       <c r="A67" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D67" s="8" t="s">
-        <v>39</v>
+      <c r="D67" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="E67" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="75">
+    <row r="68" spans="1:5" ht="150">
       <c r="A68" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D68" s="8" t="s">
-        <v>41</v>
+        <v>6</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="135">
+    <row r="69" spans="1:5" ht="75">
       <c r="A69" s="3">
+        <v>12</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E69" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="90">
+      <c r="A70" s="3">
+        <v>12</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E70" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="75">
+      <c r="A71" s="3">
+        <v>12</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E71" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="75">
+      <c r="A72" s="3">
+        <v>12</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E72" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="135">
+      <c r="A73" s="3">
         <v>14</v>
       </c>
-      <c r="B69" s="8" t="s">
+      <c r="B73" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C69" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D69" s="10" t="s">
+      <c r="C73" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E69" s="8" t="s">
+      <c r="E73" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="30">
-      <c r="A70" s="3">
+    <row r="74" spans="1:5" ht="30">
+      <c r="A74" s="3">
         <v>14</v>
       </c>
-      <c r="B70" s="8" t="s">
+      <c r="B74" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C74" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D70" s="8" t="s">
+      <c r="D74" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E70" s="8" t="s">
+      <c r="E74" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="75">
+      <c r="A75" s="3">
+        <v>14</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E75" s="8" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>